<commit_message>
Deploying to main from @ electrified/rcbus-opl3@d74fe93393cb5c20bd77984a46315af28695b014 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/rcbus-opl3-bom.xlsx
+++ b/BoM/Costs/rcbus-opl3-bom.xlsx
@@ -516,7 +516,7 @@
     <t>Date:</t>
   </si>
   <si>
-    <t>2025-09-29</t>
+    <t>2025-10-01</t>
   </si>
   <si>
     <t>KiCad Version:</t>
@@ -609,7 +609,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2025-09-29 21:03:23</t>
+    <t>2025-10-01 20:52:51</t>
   </si>
   <si>
     <t>KiCost® v1.1.20 + KiBot v1.8.4</t>

</xml_diff>

<commit_message>
Deploying to main from @ electrified/rcbus-opl3@ca335f471b0cc053c0f7ada637c7f1deac17d0b8 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/rcbus-opl3-bom.xlsx
+++ b/BoM/Costs/rcbus-opl3-bom.xlsx
@@ -166,7 +166,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="150">
   <si>
     <t>Row</t>
   </si>
@@ -252,231 +252,192 @@
     <t>3</t>
   </si>
   <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>10nF</t>
+    <t>C1 C6 C7 C12 C19</t>
+  </si>
+  <si>
+    <t>0.1uF</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
   <si>
     <t>4</t>
   </si>
   <si>
-    <t>C1 C3 C6 C7 C12 C19</t>
-  </si>
-  <si>
-    <t>0.1uF</t>
+    <t>C_Polarized_Small</t>
+  </si>
+  <si>
+    <t>C8 C15 C16</t>
+  </si>
+  <si>
+    <t>10uF</t>
+  </si>
+  <si>
+    <t>CP_Elec_6.3x5.8</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>100uF</t>
+  </si>
+  <si>
+    <t>CP_Elec_6.3x7.7</t>
   </si>
   <si>
     <t>6</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>C_Polarized_Small</t>
-  </si>
-  <si>
-    <t>C15 C16</t>
-  </si>
-  <si>
-    <t>10uf</t>
-  </si>
-  <si>
-    <t>CP_Elec_5x5.9</t>
-  </si>
-  <si>
-    <t>C4 C5</t>
-  </si>
-  <si>
-    <t>10uF</t>
-  </si>
-  <si>
-    <t>C_1206_3216Metric</t>
+    <t>AudioJack3_SwitchTR</t>
+  </si>
+  <si>
+    <t>CON1</t>
+  </si>
+  <si>
+    <t>SJ1-3523N</t>
+  </si>
+  <si>
+    <t>Headphone_Jack_3.5mm_5_pin</t>
+  </si>
+  <si>
+    <t>CP1-3523N-ND</t>
+  </si>
+  <si>
+    <t>Connectors, Interconnects</t>
+  </si>
+  <si>
+    <t>Barrel - Audio Connectors</t>
+  </si>
+  <si>
+    <t>https://www.cui.com/product/resource/digikeypdf/sj1-352xn_series.pdf</t>
+  </si>
+  <si>
+    <t>/product-detail/en/cui-inc/SJ1-3523N/CP1-3523N-ND/738689</t>
   </si>
   <si>
     <t>7</t>
   </si>
   <si>
-    <t>C8</t>
+    <t>Conn_02x06_Odd_Even</t>
+  </si>
+  <si>
+    <t>JP1</t>
+  </si>
+  <si>
+    <t>BASE ADDRESS</t>
+  </si>
+  <si>
+    <t>PinHeader_2x06_P2.54mm_Vertical</t>
   </si>
   <si>
     <t>8</t>
   </si>
   <si>
-    <t>AudioJack3_SwitchTR</t>
-  </si>
-  <si>
-    <t>CON1</t>
-  </si>
-  <si>
-    <t>SJ1-3523N</t>
-  </si>
-  <si>
-    <t>Headphone_Jack_3.5mm_5_pin</t>
-  </si>
-  <si>
-    <t>CP1-3523N-ND</t>
-  </si>
-  <si>
-    <t>Connectors, Interconnects</t>
-  </si>
-  <si>
-    <t>Barrel - Audio Connectors</t>
-  </si>
-  <si>
-    <t>https://www.cui.com/product/resource/digikeypdf/sj1-352xn_series.pdf</t>
-  </si>
-  <si>
-    <t>/product-detail/en/cui-inc/SJ1-3523N/CP1-3523N-ND/738689</t>
+    <t>Conn_01x39</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>RC2014 BUS</t>
+  </si>
+  <si>
+    <t>PinHeader_1x39_P2.54mm_Vertical</t>
   </si>
   <si>
     <t>9</t>
   </si>
   <si>
-    <t>Conn_02x06_Odd_Even</t>
-  </si>
-  <si>
-    <t>JP1</t>
-  </si>
-  <si>
-    <t>BASE ADDRESS</t>
-  </si>
-  <si>
-    <t>PinHeader_2x06_P2.54mm_Vertical</t>
+    <t>R</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>R_0603_1608Metric</t>
   </si>
   <si>
     <t>10</t>
   </si>
   <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>L2</t>
-  </si>
-  <si>
-    <t>33uH</t>
-  </si>
-  <si>
-    <t>L_0603_1608Metric</t>
+    <t>R8 R9</t>
+  </si>
+  <si>
+    <t>100</t>
   </si>
   <si>
     <t>11</t>
   </si>
   <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>BLM18PG221SN1D</t>
+    <t>R_Small</t>
+  </si>
+  <si>
+    <t>R1 R2 R3 R4 R5 R6 R10 R11</t>
+  </si>
+  <si>
+    <t>10K</t>
   </si>
   <si>
     <t>12</t>
   </si>
   <si>
-    <t>Conn_01x39</t>
-  </si>
-  <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>RC2014 BUS</t>
-  </si>
-  <si>
-    <t>PinHeader_1x39_P2.54mm_Vertical</t>
+    <t>74HCT688</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>SOIC-20W_7.5x12.8mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>https://www.ti.com/lit/ds/symlink/cd54hc688.pdf</t>
   </si>
   <si>
     <t>13</t>
   </si>
   <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>R7</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>R_0603_1608Metric</t>
+    <t>TL074</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>SOIC-14_3.9x8.7mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>http://www.ti.com/lit/ds/symlink/tl071.pdf</t>
   </si>
   <si>
     <t>14</t>
   </si>
   <si>
-    <t>R8 R9</t>
-  </si>
-  <si>
-    <t>100</t>
+    <t>YAC512</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>SOP-16_4.55x10.3mm_P1.27mm</t>
   </si>
   <si>
     <t>15</t>
   </si>
   <si>
-    <t>R_Small</t>
-  </si>
-  <si>
-    <t>R1 R2 R3 R4 R5 R6 R10 R11</t>
-  </si>
-  <si>
-    <t>10K</t>
+    <t>YMF262</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>SOP-24_7.5x15.4mm_P1.27mm</t>
   </si>
   <si>
     <t>16</t>
   </si>
   <si>
-    <t>74HCT688</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>SOIC-20W_7.5x12.8mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>https://www.ti.com/lit/ds/symlink/cd54hc688.pdf</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>TL074</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>SOIC-14_3.9x8.7mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>http://www.ti.com/lit/ds/symlink/tl071.pdf</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>YAC512</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>SOP-16_4.55x10.3mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>YMF262</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>SOP-24_7.5x15.4mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
     <t>ASV-xxxMHz</t>
   </si>
   <si>
@@ -531,7 +492,7 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>36 (33 SMD/ 3 THT)</t>
+    <t>31 (28 SMD/ 3 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
@@ -576,9 +537,6 @@
     <t>Generic connector, double row, 02x06, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
-    <t>Inductor</t>
-  </si>
-  <si>
     <t>Generic connector, single row, 01x39, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
@@ -609,7 +567,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2025-10-01 20:52:51</t>
+    <t>2025-10-01 23:05:56</t>
   </si>
   <si>
     <t>KiCost® v1.1.20 + KiBot v1.8.4</t>
@@ -1387,7 +1345,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P28"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1416,7 +1374,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1434,55 +1392,55 @@
     </row>
     <row r="2" spans="1:16">
       <c r="C2" s="2" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="F2" s="3">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="C3" s="2" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="C4" s="2" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="C5" s="2" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1490,16 +1448,16 @@
     </row>
     <row r="6" spans="1:16">
       <c r="C6" s="2" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="F6" s="3">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -1672,7 +1630,7 @@
         <v>21</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>22</v>
@@ -1704,25 +1662,25 @@
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>22</v>
@@ -1754,13 +1712,13 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>36</v>
@@ -1772,7 +1730,7 @@
         <v>38</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>22</v>
@@ -1802,27 +1760,27 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" ht="30" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>22</v>
@@ -1830,23 +1788,23 @@
       <c r="I14" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="J14" s="9" t="s">
-        <v>17</v>
+      <c r="J14" s="11" t="s">
+        <v>44</v>
       </c>
       <c r="K14" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="L14" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="M14" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="N14" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="O14" s="9" t="s">
-        <v>17</v>
+      <c r="L14" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="M14" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="N14" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="O14" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="P14" s="9" t="s">
         <v>17</v>
@@ -1854,22 +1812,22 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="5" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>16</v>
@@ -1902,24 +1860,24 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="30" customHeight="1">
+    <row r="16" spans="1:16">
       <c r="A16" s="8" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>16</v>
@@ -1930,23 +1888,23 @@
       <c r="I16" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="J16" s="11" t="s">
-        <v>49</v>
+      <c r="J16" s="9" t="s">
+        <v>17</v>
       </c>
       <c r="K16" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="L16" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="M16" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="N16" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="O16" s="11" t="s">
-        <v>53</v>
+      <c r="L16" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M16" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="N16" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="O16" s="9" t="s">
+        <v>17</v>
       </c>
       <c r="P16" s="9" t="s">
         <v>17</v>
@@ -1954,22 +1912,22 @@
     </row>
     <row r="17" spans="1:16">
       <c r="A17" s="5" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>16</v>
@@ -2004,7 +1962,7 @@
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="8" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>17</v>
@@ -2013,16 +1971,16 @@
         <v>60</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F18" s="10" t="s">
         <v>63</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>22</v>
@@ -2054,25 +2012,25 @@
     </row>
     <row r="19" spans="1:16">
       <c r="A19" s="5" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>63</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>22</v>
@@ -2104,22 +2062,22 @@
     </row>
     <row r="20" spans="1:16">
       <c r="A20" s="8" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>16</v>
@@ -2127,8 +2085,8 @@
       <c r="H20" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I20" s="9" t="s">
-        <v>23</v>
+      <c r="I20" s="10" t="s">
+        <v>75</v>
       </c>
       <c r="J20" s="9" t="s">
         <v>17</v>
@@ -2154,22 +2112,22 @@
     </row>
     <row r="21" spans="1:16">
       <c r="A21" s="5" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>16</v>
@@ -2177,8 +2135,8 @@
       <c r="H21" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I21" s="6" t="s">
-        <v>23</v>
+      <c r="I21" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="J21" s="6" t="s">
         <v>17</v>
@@ -2204,31 +2162,31 @@
     </row>
     <row r="22" spans="1:16">
       <c r="A22" s="8" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="H22" s="8" t="s">
         <v>22</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="J22" s="9" t="s">
         <v>17</v>
@@ -2254,31 +2212,31 @@
     </row>
     <row r="23" spans="1:16">
       <c r="A23" s="5" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>22</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="J23" s="6" t="s">
         <v>17</v>
@@ -2304,22 +2262,22 @@
     </row>
     <row r="24" spans="1:16">
       <c r="A24" s="8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>16</v>
@@ -2328,7 +2286,7 @@
         <v>22</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="J24" s="9" t="s">
         <v>17</v>
@@ -2349,206 +2307,6 @@
         <v>17</v>
       </c>
       <c r="P24" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16">
-      <c r="A25" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K25" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L25" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="M25" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="N25" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="O25" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="P25" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16">
-      <c r="A26" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H26" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="I26" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="J26" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="K26" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="L26" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="M26" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="N26" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="O26" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="P26" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16">
-      <c r="A27" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I27" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J27" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K27" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L27" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="M27" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="N27" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="O27" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="P27" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16">
-      <c r="A28" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H28" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="I28" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="J28" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="K28" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="L28" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="M28" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="N28" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="O28" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="P28" s="9" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2564,7 +2322,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="9" ySplit="9" topLeftCell="J10" activePane="bottomRight" state="frozen"/>
@@ -2576,7 +2334,7 @@
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="61.7109375" customWidth="1" outlineLevel="2"/>
     <col min="4" max="4" width="42.7109375" customWidth="1" outlineLevel="2"/>
     <col min="5" max="5" width="11.7109375" customWidth="1" outlineLevel="1"/>
@@ -2588,7 +2346,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2598,13 +2356,13 @@
     </row>
     <row r="2" spans="1:9">
       <c r="D2" s="2" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="I2" s="12">
         <v>1</v>
@@ -2612,13 +2370,13 @@
     </row>
     <row r="3" spans="1:9">
       <c r="D3" s="2" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="I3" s="14">
         <f>TotalCost/BoardQty</f>
@@ -2627,38 +2385,38 @@
     </row>
     <row r="4" spans="1:9">
       <c r="D4" s="2" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="I4" s="15">
-        <f>SUM(I10:I29)</f>
+        <f>SUM(I10:I25)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="D5" s="2" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="D6" s="2" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="16" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
@@ -2683,19 +2441,19 @@
         <v>5</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -2706,7 +2464,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>21</v>
@@ -2728,7 +2486,7 @@
         <v>26</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="D11" s="18" t="s">
         <v>21</v>
@@ -2750,14 +2508,14 @@
         <v>29</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>21</v>
       </c>
       <c r="G12" s="18">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*5,1)</f>
+        <v>5</v>
       </c>
       <c r="I12" s="19">
         <f>IF(AND(ISNUMBER(G12),ISNUMBER(H12)),G12*H12,"")</f>
@@ -2766,20 +2524,20 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="18" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="G13" s="18">
-        <f>CEILING(BoardQty*6,1)</f>
-        <v>6</v>
+        <f>CEILING(BoardQty*3,1)</f>
+        <v>3</v>
       </c>
       <c r="I13" s="19">
         <f>IF(AND(ISNUMBER(G13),ISNUMBER(H13)),G13*H13,"")</f>
@@ -2794,54 +2552,60 @@
         <v>37</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>38</v>
       </c>
       <c r="G14" s="18">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="I14" s="19">
         <f>IF(AND(ISNUMBER(G14),ISNUMBER(H14)),G14*H14,"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" ht="30" customHeight="1">
       <c r="A15" s="18" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>41</v>
+        <v>43</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>42</v>
       </c>
       <c r="G15" s="18">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="I15" s="19">
         <f>IF(AND(ISNUMBER(G15),ISNUMBER(H15)),G15*H15,"")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" ht="45" customHeight="1">
       <c r="A16" s="18" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="G16" s="18">
         <f>BoardQty*1</f>
@@ -2854,22 +2618,16 @@
     </row>
     <row r="17" spans="1:9" ht="30" customHeight="1">
       <c r="A17" s="18" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="F17" s="18" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="G17" s="18">
         <f>BoardQty*1</f>
@@ -2880,18 +2638,18 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="45" customHeight="1">
+    <row r="18" spans="1:9">
       <c r="A18" s="18" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G18" s="18">
         <f>BoardQty*1</f>
@@ -2904,20 +2662,20 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="18" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>63</v>
       </c>
       <c r="G19" s="18">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="I19" s="19">
         <f>IF(AND(ISNUMBER(G19),ISNUMBER(H19)),G19*H19,"")</f>
@@ -2926,38 +2684,41 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="18" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>63</v>
       </c>
       <c r="G20" s="18">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*8,1)</f>
+        <v>8</v>
       </c>
       <c r="I20" s="19">
         <f>IF(AND(ISNUMBER(G20),ISNUMBER(H20)),G20*H20,"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="30" customHeight="1">
+    <row r="21" spans="1:9">
       <c r="A21" s="18" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>71</v>
+        <v>74</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>75</v>
       </c>
       <c r="G21" s="18">
         <f>BoardQty*1</f>
@@ -2968,18 +2729,21 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" ht="30" customHeight="1">
       <c r="A22" s="18" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>76</v>
+        <v>79</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>80</v>
       </c>
       <c r="G22" s="18">
         <f>BoardQty*1</f>
@@ -2992,20 +2756,17 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="18" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="C23" s="18" t="s">
-        <v>138</v>
+        <v>82</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="G23" s="18">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="I23" s="19">
         <f>IF(AND(ISNUMBER(G23),ISNUMBER(H23)),G23*H23,"")</f>
@@ -3014,20 +2775,17 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="18" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>139</v>
+        <v>86</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="G24" s="18">
-        <f>CEILING(BoardQty*8,1)</f>
-        <v>8</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="I24" s="19">
         <f>IF(AND(ISNUMBER(G24),ISNUMBER(H24)),G24*H24,"")</f>
@@ -3036,19 +2794,19 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="18" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F25" s="18" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="G25" s="18">
         <f>BoardQty*1</f>
@@ -3059,105 +2817,17 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="30" customHeight="1">
-      <c r="A26" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="B26" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="F26" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="G26" s="18">
-        <f>BoardQty*1</f>
-        <v>1</v>
-      </c>
-      <c r="I26" s="19">
-        <f>IF(AND(ISNUMBER(G26),ISNUMBER(H26)),G26*H26,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="B27" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="D27" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="G27" s="18">
-        <f>BoardQty*1</f>
-        <v>1</v>
-      </c>
-      <c r="I27" s="19">
-        <f>IF(AND(ISNUMBER(G27),ISNUMBER(H27)),G27*H27,"")</f>
-        <v/>
-      </c>
-    </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="B28" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="D28" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="G28" s="18">
-        <f>BoardQty*1</f>
-        <v>1</v>
-      </c>
-      <c r="I28" s="19">
-        <f>IF(AND(ISNUMBER(G28),ISNUMBER(H28)),G28*H28,"")</f>
-        <v/>
+      <c r="A28" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="B29" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="D29" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="F29" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="G29" s="18">
-        <f>BoardQty*1</f>
-        <v>1</v>
-      </c>
-      <c r="I29" s="19">
-        <f>IF(AND(ISNUMBER(G29),ISNUMBER(H29)),G29*H29,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="B32" s="21" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="22" t="s">
-        <v>148</v>
+      <c r="A29" s="22" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -3245,30 +2915,10 @@
       <formula>AND(ISBLANK(F25),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G26">
-    <cfRule type="expression" dxfId="0" priority="17">
-      <formula>AND(ISBLANK(F26),TRUE())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G27">
-    <cfRule type="expression" dxfId="0" priority="18">
-      <formula>AND(ISBLANK(F27),TRUE())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G28">
-    <cfRule type="expression" dxfId="0" priority="19">
-      <formula>AND(ISBLANK(F28),TRUE())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G29">
-    <cfRule type="expression" dxfId="0" priority="20">
-      <formula>AND(ISBLANK(F29),TRUE())</formula>
-    </cfRule>
-  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F25" r:id="rId1"/>
-    <hyperlink ref="F26" r:id="rId2"/>
-    <hyperlink ref="F29" r:id="rId3"/>
+    <hyperlink ref="F21" r:id="rId1"/>
+    <hyperlink ref="F22" r:id="rId2"/>
+    <hyperlink ref="F25" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId4"/>
@@ -3289,77 +2939,77 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="23" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="6" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="24" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="25" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="26" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="27" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="28" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="29" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="30" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="31" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="32" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ electrified/rcbus-opl3@95905a1b3d61b904a2086439a003ecc01cce0db1 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/rcbus-opl3-bom.xlsx
+++ b/BoM/Costs/rcbus-opl3-bom.xlsx
@@ -166,7 +166,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="151">
   <si>
     <t>Row</t>
   </si>
@@ -267,10 +267,10 @@
     <t>C_Polarized_Small</t>
   </si>
   <si>
-    <t>C8 C15 C16</t>
-  </si>
-  <si>
-    <t>10uF</t>
+    <t>C2 C8 C15 C16</t>
+  </si>
+  <si>
+    <t>10uf</t>
   </si>
   <si>
     <t>CP_Elec_6.3x5.8</t>
@@ -294,246 +294,249 @@
     <t>CON1</t>
   </si>
   <si>
+    <t>3.5mm jack</t>
+  </si>
+  <si>
+    <t>Headphone_Jack_3.5mm_5_pin</t>
+  </si>
+  <si>
+    <t>CP1-3523N-ND</t>
+  </si>
+  <si>
+    <t>Connectors, Interconnects</t>
+  </si>
+  <si>
+    <t>Barrel - Audio Connectors</t>
+  </si>
+  <si>
+    <t>https://www.cui.com/product/resource/digikeypdf/sj1-352xn_series.pdf</t>
+  </si>
+  <si>
+    <t>/product-detail/en/cui-inc/SJ1-3523N/CP1-3523N-ND/738689</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Conn_02x06_Odd_Even</t>
+  </si>
+  <si>
+    <t>JP1</t>
+  </si>
+  <si>
+    <t>BASE ADDRESS</t>
+  </si>
+  <si>
+    <t>PinHeader_2x06_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Conn_01x39</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>RC2014 BUS</t>
+  </si>
+  <si>
+    <t>PinHeader_1x39_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>R_0603_1608Metric</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>R8 R9</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>R_Small</t>
+  </si>
+  <si>
+    <t>R1 R2 R3 R4 R5 R6 R10 R11</t>
+  </si>
+  <si>
+    <t>10K</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>74HCT688</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>SOIC-20W_7.5x12.8mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>https://www.ti.com/lit/ds/symlink/cd54hc688.pdf</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>TL074</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>SOIC-14_3.9x8.7mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>http://www.ti.com/lit/ds/symlink/tl071.pdf</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>YAC512</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>SOP-16_4.55x10.3mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>YMF262</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>SOP-24_7.5x15.4mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>ASV-xxxMHz</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>14.3181MHz</t>
+  </si>
+  <si>
+    <t>Oscillator_SMD_Abracon_ASV-4Pin_7.0x5.1mm</t>
+  </si>
+  <si>
+    <t>http://www.abracon.com/Oscillators/ASV.pdf</t>
+  </si>
+  <si>
+    <t>KiBot Bill of Materials</t>
+  </si>
+  <si>
+    <t>Schematic:</t>
+  </si>
+  <si>
+    <t>rcbus-opl3</t>
+  </si>
+  <si>
+    <t>Variant:</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>Revision:</t>
+  </si>
+  <si>
+    <t>0.0.1</t>
+  </si>
+  <si>
+    <t>Date:</t>
+  </si>
+  <si>
+    <t>2025-10-04</t>
+  </si>
+  <si>
+    <t>KiCad Version:</t>
+  </si>
+  <si>
+    <t>9.0.1+1</t>
+  </si>
+  <si>
+    <t>Component Groups:</t>
+  </si>
+  <si>
+    <t>Component Count:</t>
+  </si>
+  <si>
+    <t>32 (29 SMD/ 3 THT)</t>
+  </si>
+  <si>
+    <t>Fitted Components:</t>
+  </si>
+  <si>
+    <t>Number of PCBs:</t>
+  </si>
+  <si>
+    <t>Total Components:</t>
+  </si>
+  <si>
+    <t>Global Part Info</t>
+  </si>
+  <si>
+    <t>Manf</t>
+  </si>
+  <si>
+    <t>Manf#</t>
+  </si>
+  <si>
+    <t>Build Quantity</t>
+  </si>
+  <si>
+    <t>Unit$</t>
+  </si>
+  <si>
+    <t>Ext$</t>
+  </si>
+  <si>
+    <t>Unpolarized capacitor, small symbol</t>
+  </si>
+  <si>
+    <t>Polarized capacitor, small symbol</t>
+  </si>
+  <si>
+    <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
+  </si>
+  <si>
+    <t>CUI Inc.</t>
+  </si>
+  <si>
     <t>SJ1-3523N</t>
   </si>
   <si>
-    <t>Headphone_Jack_3.5mm_5_pin</t>
-  </si>
-  <si>
-    <t>CP1-3523N-ND</t>
-  </si>
-  <si>
-    <t>Connectors, Interconnects</t>
-  </si>
-  <si>
-    <t>Barrel - Audio Connectors</t>
-  </si>
-  <si>
-    <t>https://www.cui.com/product/resource/digikeypdf/sj1-352xn_series.pdf</t>
-  </si>
-  <si>
-    <t>/product-detail/en/cui-inc/SJ1-3523N/CP1-3523N-ND/738689</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>Conn_02x06_Odd_Even</t>
-  </si>
-  <si>
-    <t>JP1</t>
-  </si>
-  <si>
-    <t>BASE ADDRESS</t>
-  </si>
-  <si>
-    <t>PinHeader_2x06_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>Conn_01x39</t>
-  </si>
-  <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>RC2014 BUS</t>
-  </si>
-  <si>
-    <t>PinHeader_1x39_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>R7</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>R_0603_1608Metric</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>R8 R9</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>R_Small</t>
-  </si>
-  <si>
-    <t>R1 R2 R3 R4 R5 R6 R10 R11</t>
-  </si>
-  <si>
-    <t>10K</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>74HCT688</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>SOIC-20W_7.5x12.8mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>https://www.ti.com/lit/ds/symlink/cd54hc688.pdf</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>TL074</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>SOIC-14_3.9x8.7mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>http://www.ti.com/lit/ds/symlink/tl071.pdf</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>YAC512</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>SOP-16_4.55x10.3mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>YMF262</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>SOP-24_7.5x15.4mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>ASV-xxxMHz</t>
-  </si>
-  <si>
-    <t>Y1</t>
-  </si>
-  <si>
-    <t>SG-8002CA</t>
-  </si>
-  <si>
-    <t>Oscillator_SMD_Abracon_ASV-4Pin_7.0x5.1mm</t>
-  </si>
-  <si>
-    <t>http://www.abracon.com/Oscillators/ASV.pdf</t>
-  </si>
-  <si>
-    <t>KiBot Bill of Materials</t>
-  </si>
-  <si>
-    <t>Schematic:</t>
-  </si>
-  <si>
-    <t>rcbus-opl3</t>
-  </si>
-  <si>
-    <t>Variant:</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>Revision:</t>
-  </si>
-  <si>
-    <t>0.0.1</t>
-  </si>
-  <si>
-    <t>Date:</t>
-  </si>
-  <si>
-    <t>2025-10-01</t>
-  </si>
-  <si>
-    <t>KiCad Version:</t>
-  </si>
-  <si>
-    <t>9.0.1+1</t>
-  </si>
-  <si>
-    <t>Component Groups:</t>
-  </si>
-  <si>
-    <t>Component Count:</t>
-  </si>
-  <si>
-    <t>31 (28 SMD/ 3 THT)</t>
-  </si>
-  <si>
-    <t>Fitted Components:</t>
-  </si>
-  <si>
-    <t>Number of PCBs:</t>
-  </si>
-  <si>
-    <t>Total Components:</t>
-  </si>
-  <si>
-    <t>Global Part Info</t>
-  </si>
-  <si>
-    <t>Manf</t>
-  </si>
-  <si>
-    <t>Manf#</t>
-  </si>
-  <si>
-    <t>Build Quantity</t>
-  </si>
-  <si>
-    <t>Unit$</t>
-  </si>
-  <si>
-    <t>Ext$</t>
-  </si>
-  <si>
-    <t>Unpolarized capacitor, small symbol</t>
-  </si>
-  <si>
-    <t>Polarized capacitor, small symbol</t>
-  </si>
-  <si>
-    <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
-  </si>
-  <si>
-    <t>CUI Inc.</t>
-  </si>
-  <si>
     <t>Generic connector, double row, 02x06, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
@@ -567,7 +570,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2025-10-01 23:05:56</t>
+    <t>2025-10-04 22:33:57</t>
   </si>
   <si>
     <t>KiCost® v1.1.20 + KiBot v1.8.4</t>
@@ -1457,7 +1460,7 @@
         <v>111</v>
       </c>
       <c r="F6" s="3">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -1680,7 +1683,7 @@
         <v>35</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>22</v>
@@ -2362,7 +2365,7 @@
         <v>97</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I2" s="12">
         <v>1</v>
@@ -2376,7 +2379,7 @@
         <v>99</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I3" s="14">
         <f>TotalCost/BoardQty</f>
@@ -2391,7 +2394,7 @@
         <v>101</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I4" s="15">
         <f>SUM(I10:I25)</f>
@@ -2536,8 +2539,8 @@
         <v>35</v>
       </c>
       <c r="G13" s="18">
-        <f>CEILING(BoardQty*3,1)</f>
-        <v>3</v>
+        <f>CEILING(BoardQty*4,1)</f>
+        <v>4</v>
       </c>
       <c r="I13" s="19">
         <f>IF(AND(ISNUMBER(G13),ISNUMBER(H13)),G13*H13,"")</f>
@@ -2583,7 +2586,7 @@
         <v>121</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>42</v>
+        <v>122</v>
       </c>
       <c r="G15" s="18">
         <f>BoardQty*1</f>
@@ -2602,7 +2605,7 @@
         <v>52</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>53</v>
@@ -2624,7 +2627,7 @@
         <v>57</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D17" s="18" t="s">
         <v>58</v>
@@ -2646,7 +2649,7 @@
         <v>62</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D18" s="18" t="s">
         <v>63</v>
@@ -2668,7 +2671,7 @@
         <v>66</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>63</v>
@@ -2690,7 +2693,7 @@
         <v>70</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>63</v>
@@ -2712,7 +2715,7 @@
         <v>72</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D21" s="18" t="s">
         <v>74</v>
@@ -2737,7 +2740,7 @@
         <v>77</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D22" s="18" t="s">
         <v>79</v>
@@ -2800,7 +2803,7 @@
         <v>92</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>93</v>
@@ -2819,15 +2822,15 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="20" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="22" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -2939,77 +2942,77 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="23" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="24" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="25" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="26" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="27" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="28" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="29" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="30" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="31" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="32" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ electrified/rcbus-opl3@584da4a1b422c01a1dd6591974515cd0858dd859 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/rcbus-opl3-bom.xlsx
+++ b/BoM/Costs/rcbus-opl3-bom.xlsx
@@ -477,7 +477,7 @@
     <t>Date:</t>
   </si>
   <si>
-    <t>2025-10-04</t>
+    <t>2025-10-05</t>
   </si>
   <si>
     <t>KiCad Version:</t>
@@ -570,7 +570,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2025-10-04 22:33:57</t>
+    <t>2025-10-05 23:06:54</t>
   </si>
   <si>
     <t>KiCost® v1.1.20 + KiBot v1.8.4</t>

</xml_diff>

<commit_message>
Deploying to main from @ electrified/rcbus-opl3@42ce7c760070e2171aef10dfe149ca65f88f18a5 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/rcbus-opl3-bom.xlsx
+++ b/BoM/Costs/rcbus-opl3-bom.xlsx
@@ -477,7 +477,7 @@
     <t>Date:</t>
   </si>
   <si>
-    <t>2025-10-05</t>
+    <t>2025-10-06</t>
   </si>
   <si>
     <t>KiCad Version:</t>
@@ -570,7 +570,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2025-10-05 23:06:54</t>
+    <t>2025-10-06 23:48:34</t>
   </si>
   <si>
     <t>KiCost® v1.1.20 + KiBot v1.8.4</t>

</xml_diff>

<commit_message>
Deploying to main from @ electrified/rcbus-opl3@749e160d32f702c867f67f7984cd714a9df6dd66 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/rcbus-opl3-bom.xlsx
+++ b/BoM/Costs/rcbus-opl3-bom.xlsx
@@ -477,7 +477,7 @@
     <t>Date:</t>
   </si>
   <si>
-    <t>2025-10-06</t>
+    <t>2025-10-07</t>
   </si>
   <si>
     <t>KiCad Version:</t>
@@ -570,7 +570,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2025-10-06 23:48:34</t>
+    <t>2025-10-07 23:46:38</t>
   </si>
   <si>
     <t>KiCost® v1.1.20 + KiBot v1.8.4</t>

</xml_diff>

<commit_message>
Deploying to main from @ electrified/rcbus-opl3@bf3798d9d67c8703c79c41f51a896f3b0ec971bf 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/rcbus-opl3-bom.xlsx
+++ b/BoM/Costs/rcbus-opl3-bom.xlsx
@@ -477,7 +477,7 @@
     <t>Date:</t>
   </si>
   <si>
-    <t>2025-10-07</t>
+    <t>2025-10-08</t>
   </si>
   <si>
     <t>KiCad Version:</t>
@@ -570,7 +570,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2025-10-07 23:46:38</t>
+    <t>2025-10-08 18:48:53</t>
   </si>
   <si>
     <t>KiCost® v1.1.20 + KiBot v1.8.4</t>

</xml_diff>

<commit_message>
Deploying to main from @ electrified/rcbus-opl3@76df5429c526e7a9126e9bdce83f90b253efb9f7 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/rcbus-opl3-bom.xlsx
+++ b/BoM/Costs/rcbus-opl3-bom.xlsx
@@ -166,7 +166,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="150">
   <si>
     <t>Row</t>
   </si>
@@ -225,10 +225,10 @@
     <t>C_Small</t>
   </si>
   <si>
-    <t>C11</t>
-  </si>
-  <si>
-    <t>68pf</t>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>68pF</t>
   </si>
   <si>
     <t>C_0603_1608Metric</t>
@@ -243,16 +243,16 @@
     <t>2</t>
   </si>
   <si>
-    <t>C9 C10</t>
-  </si>
-  <si>
-    <t>2.7nf</t>
+    <t>C3 C4</t>
+  </si>
+  <si>
+    <t>2.7nF</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
-    <t>C1 C6 C7 C12 C19</t>
+    <t>C2 C8 C11 C12 C13</t>
   </si>
   <si>
     <t>0.1uF</t>
@@ -267,16 +267,16 @@
     <t>C_Polarized_Small</t>
   </si>
   <si>
-    <t>C2 C8 C15 C16</t>
-  </si>
-  <si>
-    <t>10uf</t>
+    <t>C1 C6 C7 C10</t>
+  </si>
+  <si>
+    <t>10uF</t>
   </si>
   <si>
     <t>CP_Elec_6.3x5.8</t>
   </si>
   <si>
-    <t>C5</t>
+    <t>C9</t>
   </si>
   <si>
     <t>100uF</t>
@@ -351,7 +351,7 @@
     <t>R</t>
   </si>
   <si>
-    <t>R7</t>
+    <t>R1</t>
   </si>
   <si>
     <t>33</t>
@@ -363,7 +363,7 @@
     <t>10</t>
   </si>
   <si>
-    <t>R8 R9</t>
+    <t>R2 R3</t>
   </si>
   <si>
     <t>100</t>
@@ -372,10 +372,7 @@
     <t>11</t>
   </si>
   <si>
-    <t>R_Small</t>
-  </si>
-  <si>
-    <t>R1 R2 R3 R4 R5 R6 R10 R11</t>
+    <t>R4 R5 R6 R7 R8 R9 R10 R11</t>
   </si>
   <si>
     <t>10K</t>
@@ -387,51 +384,51 @@
     <t>74HCT688</t>
   </si>
   <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>SOIC-20W_7.5x12.8mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>https://www.ti.com/lit/ds/symlink/cd54hc688.pdf</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>TL074</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>SOIC-14_3.9x8.7mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>http://www.ti.com/lit/ds/symlink/tl071.pdf</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>YAC512</t>
+  </si>
+  <si>
     <t>U1</t>
   </si>
   <si>
-    <t>SOIC-20W_7.5x12.8mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>https://www.ti.com/lit/ds/symlink/cd54hc688.pdf</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>TL074</t>
+    <t>SOP-16_4.55x10.3mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>YMF262</t>
   </si>
   <si>
     <t>U4</t>
   </si>
   <si>
-    <t>SOIC-14_3.9x8.7mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>http://www.ti.com/lit/ds/symlink/tl071.pdf</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>YAC512</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>SOP-16_4.55x10.3mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>YMF262</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
     <t>SOP-24_7.5x15.4mm_P1.27mm</t>
   </si>
   <si>
@@ -477,7 +474,7 @@
     <t>Date:</t>
   </si>
   <si>
-    <t>2025-10-08</t>
+    <t>2025-10-09</t>
   </si>
   <si>
     <t>KiCad Version:</t>
@@ -546,7 +543,7 @@
     <t>Resistor</t>
   </si>
   <si>
-    <t>Resistor, small symbol</t>
+    <t>Resistor Resistor, small symbol</t>
   </si>
   <si>
     <t>8-bit magnitude comparator</t>
@@ -570,7 +567,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2025-10-08 18:48:53</t>
+    <t>2025-10-09 19:14:00</t>
   </si>
   <si>
     <t>KiCost® v1.1.20 + KiBot v1.8.4</t>
@@ -1377,7 +1374,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1395,13 +1392,13 @@
     </row>
     <row r="2" spans="1:16">
       <c r="C2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>97</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F2" s="3">
         <v>16</v>
@@ -1409,41 +1406,41 @@
     </row>
     <row r="3" spans="1:16">
       <c r="C3" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>99</v>
-      </c>
       <c r="E3" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="C4" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>101</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="C5" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1451,13 +1448,13 @@
     </row>
     <row r="6" spans="1:16">
       <c r="C6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>105</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F6" s="3">
         <v>32</v>
@@ -2021,13 +2018,13 @@
         <v>17</v>
       </c>
       <c r="C19" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="E19" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>63</v>
@@ -2065,22 +2062,22 @@
     </row>
     <row r="20" spans="1:16">
       <c r="A20" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="10" t="s">
+      <c r="D20" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="E20" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F20" s="10" t="s">
         <v>73</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>74</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>16</v>
@@ -2089,7 +2086,7 @@
         <v>22</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J20" s="9" t="s">
         <v>17</v>
@@ -2115,22 +2112,22 @@
     </row>
     <row r="21" spans="1:16">
       <c r="A21" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="7" t="s">
+      <c r="D21" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="E21" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F21" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>79</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>16</v>
@@ -2139,7 +2136,7 @@
         <v>22</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J21" s="6" t="s">
         <v>17</v>
@@ -2165,22 +2162,22 @@
     </row>
     <row r="22" spans="1:16">
       <c r="A22" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="B22" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="10" t="s">
+      <c r="D22" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="E22" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" s="10" t="s">
         <v>83</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>84</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>16</v>
@@ -2215,22 +2212,22 @@
     </row>
     <row r="23" spans="1:16">
       <c r="A23" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" s="7" t="s">
+      <c r="D23" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="E23" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F23" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>88</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>16</v>
@@ -2265,22 +2262,22 @@
     </row>
     <row r="24" spans="1:16">
       <c r="A24" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="B24" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="10" t="s">
+      <c r="D24" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="E24" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="F24" s="10" t="s">
         <v>92</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>93</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>16</v>
@@ -2289,7 +2286,7 @@
         <v>22</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J24" s="9" t="s">
         <v>17</v>
@@ -2349,7 +2346,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2359,13 +2356,13 @@
     </row>
     <row r="2" spans="1:9">
       <c r="D2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>97</v>
-      </c>
       <c r="H2" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I2" s="12">
         <v>1</v>
@@ -2373,13 +2370,13 @@
     </row>
     <row r="3" spans="1:9">
       <c r="D3" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>99</v>
-      </c>
       <c r="H3" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I3" s="14">
         <f>TotalCost/BoardQty</f>
@@ -2388,13 +2385,13 @@
     </row>
     <row r="4" spans="1:9">
       <c r="D4" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>101</v>
-      </c>
       <c r="H4" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I4" s="15">
         <f>SUM(I10:I25)</f>
@@ -2403,23 +2400,23 @@
     </row>
     <row r="5" spans="1:9">
       <c r="D5" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="D6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
@@ -2444,19 +2441,19 @@
         <v>5</v>
       </c>
       <c r="E9" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="F9" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="G9" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="H9" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="I9" s="17" t="s">
         <v>116</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -2467,7 +2464,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>21</v>
@@ -2489,7 +2486,7 @@
         <v>26</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D11" s="18" t="s">
         <v>21</v>
@@ -2511,7 +2508,7 @@
         <v>29</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>21</v>
@@ -2533,7 +2530,7 @@
         <v>34</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D13" s="18" t="s">
         <v>35</v>
@@ -2555,7 +2552,7 @@
         <v>37</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>38</v>
@@ -2577,16 +2574,16 @@
         <v>42</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>43</v>
       </c>
       <c r="E15" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="F15" s="18" t="s">
         <v>121</v>
-      </c>
-      <c r="F15" s="18" t="s">
-        <v>122</v>
       </c>
       <c r="G15" s="18">
         <f>BoardQty*1</f>
@@ -2605,7 +2602,7 @@
         <v>52</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>53</v>
@@ -2627,7 +2624,7 @@
         <v>57</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D17" s="18" t="s">
         <v>58</v>
@@ -2649,7 +2646,7 @@
         <v>62</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D18" s="18" t="s">
         <v>63</v>
@@ -2671,7 +2668,7 @@
         <v>66</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>63</v>
@@ -2687,13 +2684,13 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="18" t="s">
-        <v>70</v>
-      </c>
       <c r="C20" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>63</v>
@@ -2709,19 +2706,19 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="D21" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="B21" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="D21" s="18" t="s">
+      <c r="F21" s="18" t="s">
         <v>74</v>
-      </c>
-      <c r="F21" s="18" t="s">
-        <v>75</v>
       </c>
       <c r="G21" s="18">
         <f>BoardQty*1</f>
@@ -2734,19 +2731,19 @@
     </row>
     <row r="22" spans="1:9" ht="30" customHeight="1">
       <c r="A22" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="D22" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="C22" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="D22" s="18" t="s">
+      <c r="F22" s="18" t="s">
         <v>79</v>
-      </c>
-      <c r="F22" s="18" t="s">
-        <v>80</v>
       </c>
       <c r="G22" s="18">
         <f>BoardQty*1</f>
@@ -2759,13 +2756,13 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="18" t="s">
         <v>83</v>
-      </c>
-      <c r="B23" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>84</v>
       </c>
       <c r="G23" s="18">
         <f>BoardQty*1</f>
@@ -2778,13 +2775,13 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" s="18" t="s">
         <v>87</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="D24" s="18" t="s">
-        <v>88</v>
       </c>
       <c r="G24" s="18">
         <f>BoardQty*1</f>
@@ -2797,19 +2794,19 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B25" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="C25" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="D25" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="C25" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="D25" s="18" t="s">
+      <c r="F25" s="18" t="s">
         <v>93</v>
-      </c>
-      <c r="F25" s="18" t="s">
-        <v>94</v>
       </c>
       <c r="G25" s="18">
         <f>BoardQty*1</f>
@@ -2822,15 +2819,15 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="B28" s="21" t="s">
         <v>133</v>
-      </c>
-      <c r="B28" s="21" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2942,77 +2939,77 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="26" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="28" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="29" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="30" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="31" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="32" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ electrified/rcbus-opl3@4d18163650932ad5441b7bd8b3289f36741a7241 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/rcbus-opl3-bom.xlsx
+++ b/BoM/Costs/rcbus-opl3-bom.xlsx
@@ -225,7 +225,7 @@
     <t>C_Small</t>
   </si>
   <si>
-    <t>C5</t>
+    <t>C6</t>
   </si>
   <si>
     <t>68pF</t>
@@ -252,7 +252,7 @@
     <t>3</t>
   </si>
   <si>
-    <t>C2 C8 C11 C12 C13</t>
+    <t>C5 C8 C11 C12 C13</t>
   </si>
   <si>
     <t>0.1uF</t>
@@ -267,7 +267,7 @@
     <t>C_Polarized_Small</t>
   </si>
   <si>
-    <t>C1 C6 C7 C10</t>
+    <t>C1 C2 C7 C10</t>
   </si>
   <si>
     <t>10uF</t>
@@ -363,7 +363,7 @@
     <t>10</t>
   </si>
   <si>
-    <t>R2 R3</t>
+    <t>R3 R4</t>
   </si>
   <si>
     <t>100</t>
@@ -372,7 +372,7 @@
     <t>11</t>
   </si>
   <si>
-    <t>R4 R5 R6 R7 R8 R9 R10 R11</t>
+    <t>R2 R5 R6 R7 R8 R9 R10 R11</t>
   </si>
   <si>
     <t>10K</t>
@@ -399,24 +399,24 @@
     <t>TL074</t>
   </si>
   <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>SOIC-14_3.9x8.7mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>http://www.ti.com/lit/ds/symlink/tl071.pdf</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>YAC512</t>
+  </si>
+  <si>
     <t>U2</t>
   </si>
   <si>
-    <t>SOIC-14_3.9x8.7mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>http://www.ti.com/lit/ds/symlink/tl071.pdf</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>YAC512</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
     <t>SOP-16_4.55x10.3mm_P1.27mm</t>
   </si>
   <si>
@@ -567,7 +567,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2025-10-09 19:14:00</t>
+    <t>2025-10-09 21:11:23</t>
   </si>
   <si>
     <t>KiCost® v1.1.20 + KiBot v1.8.4</t>

</xml_diff>

<commit_message>
Deploying to main from @ electrified/rcbus-opl3@44c55904765375cbeefdfa411b2ca464d51f40a2 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/rcbus-opl3-bom.xlsx
+++ b/BoM/Costs/rcbus-opl3-bom.xlsx
@@ -474,7 +474,7 @@
     <t>Date:</t>
   </si>
   <si>
-    <t>2025-10-09</t>
+    <t>2025-10-11</t>
   </si>
   <si>
     <t>KiCad Version:</t>
@@ -567,7 +567,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2025-10-09 21:41:19</t>
+    <t>2025-10-11 13:15:53</t>
   </si>
   <si>
     <t>KiCost® v1.1.20 + KiBot v1.8.4</t>

</xml_diff>

<commit_message>
Deploying to main from @ electrified/rcbus-opl3@b421ed74cec5974dc3bbc62da0d3b0773d89e203 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/rcbus-opl3-bom.xlsx
+++ b/BoM/Costs/rcbus-opl3-bom.xlsx
@@ -166,7 +166,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="156">
   <si>
     <t>Row</t>
   </si>
@@ -276,6 +276,9 @@
     <t>CP_Elec_6.3x5.8</t>
   </si>
   <si>
+    <t>https://www.we-online.com/components/products/datasheet/875105240001.pdf</t>
+  </si>
+  <si>
     <t>C9</t>
   </si>
   <si>
@@ -420,6 +423,9 @@
     <t>SOP-16_4.55x10.3mm_P1.27mm</t>
   </si>
   <si>
+    <t>https://www.ardent-tool.com/datasheets/Yamaha_YAC512.pdf</t>
+  </si>
+  <si>
     <t>15</t>
   </si>
   <si>
@@ -432,6 +438,9 @@
     <t>SOP-24_7.5x15.4mm_P1.27mm</t>
   </si>
   <si>
+    <t>http://www.bitsavers.org/components/yamaha/YMF262_199110.pdf</t>
+  </si>
+  <si>
     <t>16</t>
   </si>
   <si>
@@ -447,7 +456,7 @@
     <t>Oscillator_SMD_Abracon_ASV-4Pin_7.0x5.1mm</t>
   </si>
   <si>
-    <t>http://www.abracon.com/Oscillators/ASV.pdf</t>
+    <t>https://4donline.ihs.com/images/VipMasterIC/IC/SCMP/SCMP-S-A0010069830/SCMP-S-A0010069830-1.pdf?hkey=6D3A4C79FDBF58556ACFDE234799DDF0</t>
   </si>
   <si>
     <t>KiBot Bill of Materials</t>
@@ -522,7 +531,13 @@
     <t>Unpolarized capacitor, small symbol</t>
   </si>
   <si>
-    <t>Polarized capacitor, small symbol</t>
+    <t>Polymer Aluminium Electrolytic Capacitor, 10 µF, 10 V, Radial Can - SMD, 0.045 ohm</t>
+  </si>
+  <si>
+    <t>875105240001</t>
+  </si>
+  <si>
+    <t>Polymer Aluminium Electrolytic Capacitor, 100 µF, 25 V, Radial Can - SMD, 0.036 ohm</t>
   </si>
   <si>
     <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
@@ -543,16 +558,19 @@
     <t>Resistor</t>
   </si>
   <si>
-    <t>Resistor Resistor, small symbol</t>
-  </si>
-  <si>
-    <t>8-bit magnitude comparator</t>
+    <t>Resistor SMD Chip Resistor, 10 kohm, ± 1%, 100 mW, 0603 [1608 Metric], Thick Film, General Purpose</t>
+  </si>
+  <si>
+    <t>Digital Comparator, 74HCT688, Magnitude, 8 Channels, 8bit, SOIC, 20 Pins</t>
   </si>
   <si>
     <t>Quad Low-Noise JFET-Input Operational Amplifiers, DIP-14/SOIC-14</t>
   </si>
   <si>
-    <t>3.3V HCMOS SMD Crystal Clock Oscillator, Abracon</t>
+    <t>2-Channel floating D/A converter</t>
+  </si>
+  <si>
+    <t>Oscillator, 14.31818 MHz, 25 ppm, SMD, 7mm x 5mm, CMOS / TTL, 5 V</t>
   </si>
   <si>
     <t>Board Qty:</t>
@@ -567,7 +585,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2025-10-11 13:15:53</t>
+    <t>2025-10-11 13:57:18</t>
   </si>
   <si>
     <t>KiCost® v1.1.20 + KiBot v1.8.4</t>
@@ -1362,7 +1380,7 @@
     <col min="6" max="6" width="46.7109375" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
-    <col min="9" max="9" width="52.7109375" customWidth="1"/>
+    <col min="9" max="9" width="60.7109375" customWidth="1"/>
     <col min="10" max="10" width="21.7109375" customWidth="1"/>
     <col min="11" max="11" width="13.7109375" customWidth="1"/>
     <col min="12" max="12" width="30.7109375" customWidth="1"/>
@@ -1374,7 +1392,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1392,13 +1410,13 @@
     </row>
     <row r="2" spans="1:16">
       <c r="C2" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F2" s="3">
         <v>16</v>
@@ -1406,41 +1424,41 @@
     </row>
     <row r="3" spans="1:16">
       <c r="C3" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="C4" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="C5" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1448,13 +1466,13 @@
     </row>
     <row r="6" spans="1:16">
       <c r="C6" s="2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="F6" s="3">
         <v>32</v>
@@ -1660,7 +1678,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" ht="30" customHeight="1">
       <c r="A12" s="8" t="s">
         <v>31</v>
       </c>
@@ -1685,8 +1703,8 @@
       <c r="H12" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="9" t="s">
-        <v>23</v>
+      <c r="I12" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="J12" s="9" t="s">
         <v>17</v>
@@ -1721,13 +1739,13 @@
         <v>32</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>16</v>
@@ -1762,22 +1780,22 @@
     </row>
     <row r="14" spans="1:16" ht="30" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>16</v>
@@ -1789,22 +1807,22 @@
         <v>23</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K14" s="9" t="s">
         <v>17</v>
       </c>
       <c r="L14" s="11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M14" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N14" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="O14" s="11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="P14" s="9" t="s">
         <v>17</v>
@@ -1812,22 +1830,22 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>16</v>
@@ -1862,22 +1880,22 @@
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>16</v>
@@ -1912,22 +1930,22 @@
     </row>
     <row r="17" spans="1:16">
       <c r="A17" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>16</v>
@@ -1962,22 +1980,22 @@
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F18" s="10" t="s">
         <v>64</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>63</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>24</v>
@@ -2012,25 +2030,25 @@
     </row>
     <row r="19" spans="1:16">
       <c r="A19" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>22</v>
@@ -2062,22 +2080,22 @@
     </row>
     <row r="20" spans="1:16">
       <c r="A20" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D20" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E20" s="10" t="s">
-        <v>71</v>
-      </c>
       <c r="F20" s="10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>16</v>
@@ -2086,7 +2104,7 @@
         <v>22</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="J20" s="9" t="s">
         <v>17</v>
@@ -2112,22 +2130,22 @@
     </row>
     <row r="21" spans="1:16">
       <c r="A21" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D21" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E21" s="7" t="s">
-        <v>76</v>
-      </c>
       <c r="F21" s="7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>16</v>
@@ -2136,7 +2154,7 @@
         <v>22</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J21" s="6" t="s">
         <v>17</v>
@@ -2162,22 +2180,22 @@
     </row>
     <row r="22" spans="1:16">
       <c r="A22" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D22" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="E22" s="10" t="s">
-        <v>81</v>
-      </c>
       <c r="F22" s="10" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>16</v>
@@ -2185,8 +2203,8 @@
       <c r="H22" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I22" s="9" t="s">
-        <v>17</v>
+      <c r="I22" s="10" t="s">
+        <v>85</v>
       </c>
       <c r="J22" s="9" t="s">
         <v>17</v>
@@ -2212,22 +2230,22 @@
     </row>
     <row r="23" spans="1:16">
       <c r="A23" s="5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>16</v>
@@ -2235,8 +2253,8 @@
       <c r="H23" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I23" s="6" t="s">
-        <v>17</v>
+      <c r="I23" s="7" t="s">
+        <v>90</v>
       </c>
       <c r="J23" s="6" t="s">
         <v>17</v>
@@ -2260,24 +2278,24 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" ht="45" customHeight="1">
       <c r="A24" s="8" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>16</v>
@@ -2286,7 +2304,7 @@
         <v>22</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="J24" s="9" t="s">
         <v>17</v>
@@ -2338,7 +2356,7 @@
     <col min="3" max="3" width="61.7109375" customWidth="1" outlineLevel="2"/>
     <col min="4" max="4" width="42.7109375" customWidth="1" outlineLevel="2"/>
     <col min="5" max="5" width="11.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="48.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="61.7109375" customWidth="1" outlineLevel="1"/>
     <col min="7" max="7" width="17.7109375" customWidth="1" outlineLevel="1"/>
     <col min="8" max="8" width="15.7109375" customWidth="1"/>
     <col min="9" max="9" width="16.7109375" customWidth="1"/>
@@ -2346,7 +2364,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2356,13 +2374,13 @@
     </row>
     <row r="2" spans="1:9">
       <c r="D2" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="I2" s="12">
         <v>1</v>
@@ -2370,13 +2388,13 @@
     </row>
     <row r="3" spans="1:9">
       <c r="D3" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="I3" s="14">
         <f>TotalCost/BoardQty</f>
@@ -2385,13 +2403,13 @@
     </row>
     <row r="4" spans="1:9">
       <c r="D4" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="I4" s="15">
         <f>SUM(I10:I25)</f>
@@ -2400,23 +2418,23 @@
     </row>
     <row r="5" spans="1:9">
       <c r="D5" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="D6" s="2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="16" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
@@ -2441,19 +2459,19 @@
         <v>5</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -2464,7 +2482,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>21</v>
@@ -2486,7 +2504,7 @@
         <v>26</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D11" s="18" t="s">
         <v>21</v>
@@ -2508,7 +2526,7 @@
         <v>29</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>21</v>
@@ -2522,7 +2540,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" ht="30" customHeight="1">
       <c r="A13" s="18" t="s">
         <v>33</v>
       </c>
@@ -2530,10 +2548,13 @@
         <v>34</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="D13" s="18" t="s">
         <v>35</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>122</v>
       </c>
       <c r="G13" s="18">
         <f>CEILING(BoardQty*4,1)</f>
@@ -2544,18 +2565,18 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" ht="30" customHeight="1">
       <c r="A14" s="18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G14" s="18">
         <f>BoardQty*1</f>
@@ -2568,22 +2589,22 @@
     </row>
     <row r="15" spans="1:9" ht="30" customHeight="1">
       <c r="A15" s="18" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="G15" s="18">
         <f>BoardQty*1</f>
@@ -2596,16 +2617,16 @@
     </row>
     <row r="16" spans="1:9" ht="45" customHeight="1">
       <c r="A16" s="18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G16" s="18">
         <f>BoardQty*1</f>
@@ -2618,16 +2639,16 @@
     </row>
     <row r="17" spans="1:9" ht="30" customHeight="1">
       <c r="A17" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G17" s="18">
         <f>BoardQty*1</f>
@@ -2640,16 +2661,16 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G18" s="18">
         <f>BoardQty*1</f>
@@ -2662,16 +2683,16 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G19" s="18">
         <f>CEILING(BoardQty*2,1)</f>
@@ -2682,18 +2703,18 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" ht="30" customHeight="1">
       <c r="A20" s="18" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G20" s="18">
         <f>CEILING(BoardQty*8,1)</f>
@@ -2704,21 +2725,21 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" ht="30" customHeight="1">
       <c r="A21" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="18" t="s">
-        <v>71</v>
-      </c>
       <c r="C21" s="18" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G21" s="18">
         <f>BoardQty*1</f>
@@ -2731,19 +2752,19 @@
     </row>
     <row r="22" spans="1:9" ht="30" customHeight="1">
       <c r="A22" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="B22" s="18" t="s">
-        <v>76</v>
-      </c>
       <c r="C22" s="18" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F22" s="18" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G22" s="18">
         <f>BoardQty*1</f>
@@ -2756,13 +2777,19 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="B23" s="18" t="s">
-        <v>81</v>
+      <c r="C23" s="18" t="s">
+        <v>133</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>83</v>
+        <v>84</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>85</v>
       </c>
       <c r="G23" s="18">
         <f>BoardQty*1</f>
@@ -2775,13 +2802,16 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="18" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>87</v>
+        <v>89</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>90</v>
       </c>
       <c r="G24" s="18">
         <f>BoardQty*1</f>
@@ -2792,21 +2822,21 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" ht="45" customHeight="1">
       <c r="A25" s="18" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F25" s="18" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G25" s="18">
         <f>BoardQty*1</f>
@@ -2819,15 +2849,15 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="20" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="22" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2916,13 +2946,16 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F21" r:id="rId1"/>
-    <hyperlink ref="F22" r:id="rId2"/>
-    <hyperlink ref="F25" r:id="rId3"/>
+    <hyperlink ref="F13" r:id="rId1"/>
+    <hyperlink ref="F21" r:id="rId2"/>
+    <hyperlink ref="F22" r:id="rId3"/>
+    <hyperlink ref="F23" r:id="rId4"/>
+    <hyperlink ref="F24" r:id="rId5"/>
+    <hyperlink ref="F25" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId4"/>
-  <legacyDrawing r:id="rId5"/>
+  <drawing r:id="rId7"/>
+  <legacyDrawing r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -2939,77 +2972,77 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="23" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="6" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="24" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="25" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="26" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="27" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="28" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="29" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="30" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="31" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="32" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>